<commit_message>
C1 integrate in same line than other Cx same value
</commit_message>
<xml_diff>
--- a/docs/_bom/bom.xlsx
+++ b/docs/_bom/bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="390" windowWidth="19815" windowHeight="8175"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ESP_MAD_RevF" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
   <si>
     <t>Qty</t>
   </si>
@@ -91,21 +91,12 @@
     <t>10uF/25/10%</t>
   </si>
   <si>
-    <t>C2, C4</t>
-  </si>
-  <si>
     <t>GRM188R61E106KA73D</t>
   </si>
   <si>
     <t>81-GRM188R61E106KA3D</t>
   </si>
   <si>
-    <t>10uF/25V/10%</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>1K(1%)</t>
   </si>
   <si>
@@ -374,6 +365,9 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>C2, C4,C1</t>
   </si>
 </sst>
 </file>
@@ -698,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -813,6 +807,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -858,12 +987,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1199,10 +1337,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1217,753 +1358,730 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7">
+        <v>1769</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G30" si="0">F2*B2</f>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="6">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0880000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.433</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="B8" s="6">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="6">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>1769</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.252</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.153</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="6">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.221</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.35099999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="6">
+        <v>2.13</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="0"/>
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="6">
+        <v>6.55</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="0"/>
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A30" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="10">
         <v>0.68</v>
       </c>
-      <c r="G2">
-        <f>F2*B2</f>
+      <c r="G30" s="11">
+        <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>0.2</v>
-      </c>
-      <c r="G3">
-        <f>F3*B3</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="G4">
-        <f>F4*B4</f>
-        <v>1.0880000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>0.18</v>
-      </c>
-      <c r="G5">
-        <f>F5*B5</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6">
-        <v>0.433</v>
-      </c>
-      <c r="G6">
-        <f>F6*B6</f>
-        <v>0.433</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="G7">
-        <f>F7*B7</f>
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="G8">
-        <f>F8*B8</f>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="G9">
-        <f>F9*B9</f>
-        <v>0.32400000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10">
-        <v>0.43</v>
-      </c>
-      <c r="G10">
-        <f>F10*B10</f>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11">
-        <v>0.252</v>
-      </c>
-      <c r="G11">
-        <f>F11*B11</f>
-        <v>0.252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12">
-        <v>0.16</v>
-      </c>
-      <c r="G12">
-        <f>F12*B12</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13">
-        <v>0.153</v>
-      </c>
-      <c r="G13">
-        <f>F13*B13</f>
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14">
-        <v>0.46</v>
-      </c>
-      <c r="G14">
-        <f>F14*B14</f>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="32" spans="1:7">
+      <c r="F32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15">
-        <v>0.221</v>
-      </c>
-      <c r="G15">
-        <f>F15*B15</f>
-        <v>0.88400000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16">
-        <v>0.43</v>
-      </c>
-      <c r="G16">
-        <f>F16*B16</f>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17">
-        <v>0.16</v>
-      </c>
-      <c r="G17">
-        <f>F17*B17</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18">
-        <v>0.81</v>
-      </c>
-      <c r="G18">
-        <f>F18*B18</f>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19">
-        <v>0.42</v>
-      </c>
-      <c r="G19">
-        <f>F19*B19</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20">
-        <v>0.72</v>
-      </c>
-      <c r="G20">
-        <f>F20*B20</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="G21">
-        <f>F21*B21</f>
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22">
-        <v>0.39</v>
-      </c>
-      <c r="G22">
-        <f>F22*B22</f>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23">
-        <v>3.3</v>
-      </c>
-      <c r="G23">
-        <f>F23*B23</f>
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24">
-        <v>0.89</v>
-      </c>
-      <c r="G24">
-        <f>F24*B24</f>
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25">
-        <v>0.49</v>
-      </c>
-      <c r="G25">
-        <f>F25*B25</f>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="G26">
-        <f>F26*B26</f>
-        <v>0.35099999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27">
-        <v>2.13</v>
-      </c>
-      <c r="G27">
-        <f>F27*B27</f>
-        <v>2.13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28">
-        <v>0.49</v>
-      </c>
-      <c r="G28">
-        <f>F28*B28</f>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29">
-        <v>6.55</v>
-      </c>
-      <c r="G29">
-        <f>F29*B29</f>
-        <v>6.55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="G30">
-        <f>F30*B30</f>
-        <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31">
-        <v>0.68</v>
-      </c>
-      <c r="G31">
-        <f>F31*B31</f>
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7">
-      <c r="F33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="2">
-        <f>SUM(G2:G32)</f>
+      <c r="G32" s="1">
+        <f>SUM(G2:G31)</f>
         <v>28.619</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for RevG Hardware
</commit_message>
<xml_diff>
--- a/docs/_bom/bom.xlsx
+++ b/docs/_bom/bom.xlsx
@@ -340,9 +340,6 @@
     <t>576-SP0503BAHTG</t>
   </si>
   <si>
-    <t>C5, C12, C17, C18</t>
-  </si>
-  <si>
     <t>R1, R2, R3, R4</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>C2, C4,C1</t>
+  </si>
+  <si>
+    <t>C12, C17, C18</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1371,10 +1371,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1401,7 +1401,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B3" s="6">
         <v>4</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="6">
         <v>4</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="6">
         <v>4</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="6">
         <v>3</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="6">
         <v>3</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="6">
         <v>3</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="F32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(G2:G31)</f>

</xml_diff>

<commit_message>
Update for Gerber RevH
</commit_message>
<xml_diff>
--- a/docs/_bom/bom.xlsx
+++ b/docs/_bom/bom.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="480" yWindow="390" windowWidth="19815" windowHeight="8175"/>
   </bookViews>
   <sheets>
-    <sheet name="ESP_MAD_RevF" sheetId="1" r:id="rId1"/>
+    <sheet name="ESP_MAD_RevH" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="120">
   <si>
     <t>Qty</t>
   </si>
@@ -25,12 +25,6 @@
     <t>Parts</t>
   </si>
   <si>
-    <t>MANUFACTURER_PART_NUMBER</t>
-  </si>
-  <si>
-    <t>MOUSER_PART_NUMBER</t>
-  </si>
-  <si>
     <t>CN1</t>
   </si>
   <si>
@@ -289,15 +283,6 @@
     <t>863-MBR120VLSFT3G</t>
   </si>
   <si>
-    <t>MLL1200S</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>506-MLL1200S</t>
-  </si>
-  <si>
     <t>MPC73831T-2ACI/OT</t>
   </si>
   <si>
@@ -355,25 +340,50 @@
     <t>C7, C14, C16</t>
   </si>
   <si>
-    <t>UNIT_PRICE</t>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>C2, C4,C1</t>
+  </si>
+  <si>
+    <t>C12, C17, C18</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>EG1213</t>
+  </si>
+  <si>
+    <t>612-EG1213</t>
+  </si>
+  <si>
+    <t>Manufacturer part Number</t>
+  </si>
+  <si>
+    <t>Mouser part number</t>
+  </si>
+  <si>
+    <t>SI2323DDS-T1-GE3</t>
+  </si>
+  <si>
+    <t>Subsitute</t>
+  </si>
+  <si>
+    <t>UNIT_PRICE (per 10 sept. 21)</t>
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>C2, C4,C1</t>
-  </si>
-  <si>
-    <t>C12, C17, C18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.000\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -692,7 +702,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -838,13 +848,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -862,7 +887,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -872,66 +897,6 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -989,19 +954,39 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1340,21 +1325,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1365,719 +1354,753 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>1769</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" ref="H2:H30" si="0">G2*B2</f>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="9">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="9">
+        <v>0.32</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="9">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.42000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="9">
+        <v>0.32</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="9">
+        <v>0.156</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="9">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="9">
+        <v>0.46</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="9">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="9">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.68100000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="9">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="9">
+        <v>0.313</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="9">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.57299999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="9">
+        <v>1.58</v>
+      </c>
+      <c r="H20" s="9">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="H22" s="9">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="9">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="9">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="0"/>
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="9">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="0"/>
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="F26" s="5"/>
+      <c r="G26" s="9">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="0"/>
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7">
-        <v>1769</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.68</v>
-      </c>
-      <c r="G2" s="8">
-        <f t="shared" ref="G2:G30" si="0">F2*B2</f>
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="6">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="8">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="6">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.0880000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.18</v>
-      </c>
-      <c r="G5" s="8">
-        <f t="shared" si="0"/>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="C27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="9">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="0"/>
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.433</v>
-      </c>
-      <c r="G6" s="8">
-        <f t="shared" si="0"/>
-        <v>0.433</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="C28" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="9">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="0"/>
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A30" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="G7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="6">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="G8" s="8">
-        <f t="shared" si="0"/>
-        <v>0.97199999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="6">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.43</v>
-      </c>
-      <c r="G9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.252</v>
-      </c>
-      <c r="G10" s="8">
-        <f t="shared" si="0"/>
-        <v>0.252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.16</v>
-      </c>
-      <c r="G11" s="8">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.153</v>
-      </c>
-      <c r="G12" s="8">
-        <f t="shared" si="0"/>
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.46</v>
-      </c>
-      <c r="G13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="6">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.221</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" si="0"/>
-        <v>0.88400000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="6">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.43</v>
-      </c>
-      <c r="G15" s="8">
-        <f t="shared" si="0"/>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0.16</v>
-      </c>
-      <c r="G16" s="8">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0.81</v>
-      </c>
-      <c r="G17" s="8">
-        <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0.42</v>
-      </c>
-      <c r="G18" s="8">
-        <f t="shared" si="0"/>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0.72</v>
-      </c>
-      <c r="G19" s="8">
-        <f t="shared" si="0"/>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="6">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="G20" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="6">
-        <v>0.39</v>
-      </c>
-      <c r="G21" s="8">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="6">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="6">
-        <v>3.3</v>
-      </c>
-      <c r="G22" s="8">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="6">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0.89</v>
-      </c>
-      <c r="G23" s="8">
-        <f t="shared" si="0"/>
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="6">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="G24" s="8">
-        <f t="shared" si="0"/>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="6">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="G25" s="8">
-        <f t="shared" si="0"/>
-        <v>0.35099999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="6">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="6">
-        <v>2.13</v>
-      </c>
-      <c r="G26" s="8">
-        <f t="shared" si="0"/>
-        <v>2.13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="6">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="G27" s="8">
-        <f t="shared" si="0"/>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="C30" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" s="6">
-        <v>6.55</v>
-      </c>
-      <c r="G28" s="8">
-        <f t="shared" si="0"/>
-        <v>6.55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="6">
-        <v>2</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="D30" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="6">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="G29" s="8">
-        <f t="shared" si="0"/>
-        <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A30" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" s="10">
-        <v>1</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0.68</v>
-      </c>
-      <c r="G30" s="11">
-        <f t="shared" si="0"/>
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="F32" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G32" s="1">
-        <f>SUM(G2:G31)</f>
-        <v>28.619</v>
+      <c r="F30" s="7"/>
+      <c r="G30" s="10">
+        <v>0.91</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="G32" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H32" s="11">
+        <f>SUM(H2:H31)</f>
+        <v>21.505000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>